<commit_message>
update README + Proben
</commit_message>
<xml_diff>
--- a/Proben.xlsx
+++ b/Proben.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
   <si>
     <t>100-115</t>
   </si>
@@ -152,79 +152,10 @@
     <t>Öl kontaminiert</t>
   </si>
   <si>
-    <t>OT_110705</t>
-  </si>
-  <si>
-    <t>OT_160805</t>
-  </si>
-  <si>
-    <t>OT_180705</t>
-  </si>
-  <si>
-    <t>MT1_050805</t>
-  </si>
-  <si>
-    <t>MT2_180805</t>
-  </si>
-  <si>
-    <t>MT3_070905</t>
-  </si>
-  <si>
-    <t>MT4_140905</t>
-  </si>
-  <si>
-    <t>MT5_230905</t>
-  </si>
-  <si>
-    <t>MT6_240905</t>
-  </si>
-  <si>
-    <t>MT7_100306</t>
-  </si>
-  <si>
-    <t>MT8_270406</t>
-  </si>
-  <si>
-    <t>ch1</t>
-  </si>
-  <si>
-    <t>ch2</t>
-  </si>
-  <si>
-    <t>ch3</t>
-  </si>
-  <si>
-    <t>Set</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>Verzeichnis</t>
-  </si>
-  <si>
     <t>Probennummer</t>
   </si>
   <si>
-    <t>tme</t>
-  </si>
-  <si>
-    <t>wav</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>son</t>
-  </si>
-  <si>
-    <t>son_long</t>
-  </si>
-  <si>
     <t>Proben</t>
-  </si>
-  <si>
-    <t>Signale</t>
   </si>
   <si>
     <t>Set - Anzahl Proben</t>
@@ -282,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -319,31 +250,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -366,19 +277,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -387,20 +295,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,68 +589,38 @@
     <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="9" width="11.42578125" style="1"/>
+    <col min="10" max="10" width="12.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="K1" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="14"/>
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="13"/>
       <c r="J2" s="2"/>
-      <c r="M2" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="14"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -780,44 +646,8 @@
       <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,34 +667,15 @@
         <v>8</v>
       </c>
       <c r="H4" s="6">
-        <f>IF(F4&lt;&gt;"",$B4,"")</f>
+        <f t="shared" ref="H4:H29" si="0">IF(F4&lt;&gt;"",$B4,"")</f>
         <v>16</v>
       </c>
       <c r="I4" s="7">
-        <f>IF(G4&lt;&gt;"",$B4,"")</f>
+        <f t="shared" ref="I4:I29" si="1">IF(G4&lt;&gt;"",$B4,"")</f>
         <v>16</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" s="6">
-        <v>400</v>
-      </c>
-      <c r="N4" s="7">
-        <v>400</v>
-      </c>
-      <c r="O4" s="9">
-        <v>4</v>
-      </c>
-      <c r="S4" s="6"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="7"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -884,34 +695,15 @@
         <v>8</v>
       </c>
       <c r="H5" s="6">
-        <f>IF(F5&lt;&gt;"",$B5,"")</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="I5" s="7">
-        <f>IF(G5&lt;&gt;"",$B5,"")</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M5" s="6">
-        <v>80</v>
-      </c>
-      <c r="N5" s="7">
-        <v>80</v>
-      </c>
-      <c r="O5" s="9">
-        <v>2</v>
-      </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="7"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -931,34 +723,15 @@
         <v>8</v>
       </c>
       <c r="H6" s="6">
-        <f>IF(F6&lt;&gt;"",$B6,"")</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="I6" s="7">
-        <f>IF(G6&lt;&gt;"",$B6,"")</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" s="6">
-        <v>82</v>
-      </c>
-      <c r="N6" s="7">
-        <v>82</v>
-      </c>
-      <c r="O6" s="9">
-        <v>4</v>
-      </c>
-      <c r="S6" s="6"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="7"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -976,43 +749,15 @@
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="6">
-        <f>IF(F7&lt;&gt;"",$B7,"")</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f>IF(G7&lt;&gt;"",$B7,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="6">
-        <v>162</v>
-      </c>
-      <c r="N7" s="7">
-        <v>162</v>
-      </c>
-      <c r="O7" s="9">
-        <v>3</v>
-      </c>
-      <c r="P7" s="1">
-        <v>162</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>162</v>
-      </c>
-      <c r="R7" s="1">
-        <v>3</v>
-      </c>
-      <c r="S7" s="6"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="7"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1032,43 +777,15 @@
         <v>8</v>
       </c>
       <c r="H8" s="6">
-        <f>IF(F8&lt;&gt;"",$B8,"")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I8" s="7">
-        <f>IF(G8&lt;&gt;"",$B8,"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="6">
-        <v>162</v>
-      </c>
-      <c r="N8" s="7">
-        <v>162</v>
-      </c>
-      <c r="O8" s="9">
-        <v>2</v>
-      </c>
-      <c r="P8" s="1">
-        <v>162</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>162</v>
-      </c>
-      <c r="R8" s="1">
-        <v>2</v>
-      </c>
-      <c r="S8" s="6"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="7"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1088,47 +805,15 @@
         <v>8</v>
       </c>
       <c r="H9" s="6">
-        <f>IF(F9&lt;&gt;"",$B9,"")</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="I9" s="7">
-        <f>IF(G9&lt;&gt;"",$B9,"")</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="6">
-        <v>162</v>
-      </c>
-      <c r="N9" s="7">
-        <v>162</v>
-      </c>
-      <c r="O9" s="9">
-        <v>2</v>
-      </c>
-      <c r="P9" s="1">
-        <v>162</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>162</v>
-      </c>
-      <c r="R9" s="1">
-        <v>2</v>
-      </c>
-      <c r="S9" s="6"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="6">
-        <v>1</v>
-      </c>
-      <c r="V9" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1148,51 +833,15 @@
         <v>8</v>
       </c>
       <c r="H10" s="6">
-        <f>IF(F10&lt;&gt;"",$B10,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I10" s="7">
-        <f>IF(G10&lt;&gt;"",$B10,"")</f>
-        <v>3</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" s="6">
-        <v>162</v>
-      </c>
-      <c r="N10" s="7">
-        <v>162</v>
-      </c>
-      <c r="O10" s="9">
-        <v>2</v>
-      </c>
-      <c r="P10" s="1">
-        <v>162</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>162</v>
-      </c>
-      <c r="R10" s="1">
-        <v>2</v>
-      </c>
-      <c r="S10" s="6">
-        <v>162</v>
-      </c>
-      <c r="T10" s="7">
-        <v>162</v>
-      </c>
-      <c r="U10" s="6">
-        <v>162</v>
-      </c>
-      <c r="V10" s="7">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1212,45 +861,17 @@
         <v>8</v>
       </c>
       <c r="H11" s="6">
-        <f>IF(F11&lt;&gt;"",$B11,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I11" s="7">
-        <f>IF(G11&lt;&gt;"",$B11,"")</f>
-        <v>3</v>
-      </c>
-      <c r="K11" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="6">
-        <v>162</v>
-      </c>
-      <c r="N11" s="7">
-        <v>162</v>
-      </c>
-      <c r="O11" s="9">
-        <v>2</v>
-      </c>
-      <c r="P11" s="1">
-        <v>162</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>162</v>
-      </c>
-      <c r="R11" s="1">
-        <v>2</v>
-      </c>
-      <c r="S11" s="6"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="7"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
@@ -1268,43 +889,15 @@
         <v>8</v>
       </c>
       <c r="H12" s="6">
-        <f>IF(F12&lt;&gt;"",$B12,"")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I12" s="7">
-        <f>IF(G12&lt;&gt;"",$B12,"")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M12" s="6">
-        <v>162</v>
-      </c>
-      <c r="N12" s="7">
-        <v>162</v>
-      </c>
-      <c r="O12" s="9">
-        <v>2</v>
-      </c>
-      <c r="P12" s="1">
-        <v>162</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>162</v>
-      </c>
-      <c r="R12" s="1">
-        <v>2</v>
-      </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="7"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1327,51 +920,15 @@
         <v>8</v>
       </c>
       <c r="H13" s="6">
-        <f>IF(F13&lt;&gt;"",$B13,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I13" s="7">
-        <f>IF(G13&lt;&gt;"",$B13,"")</f>
-        <v>3</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="6">
-        <v>233</v>
-      </c>
-      <c r="N13" s="7">
-        <v>233</v>
-      </c>
-      <c r="O13" s="9">
-        <v>3</v>
-      </c>
-      <c r="P13" s="1">
-        <v>233</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>233</v>
-      </c>
-      <c r="R13" s="1">
-        <v>3</v>
-      </c>
-      <c r="S13" s="6">
-        <v>233</v>
-      </c>
-      <c r="T13" s="7">
-        <v>233</v>
-      </c>
-      <c r="U13" s="6">
-        <v>233</v>
-      </c>
-      <c r="V13" s="7">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1392,51 +949,15 @@
         <v>8</v>
       </c>
       <c r="H14" s="6" t="str">
-        <f>IF(F14&lt;&gt;"",$B14,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I14" s="7">
-        <f>IF(G14&lt;&gt;"",$B14,"")</f>
-        <v>1</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="M14" s="11">
-        <v>233</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="O14" s="12">
-        <v>2</v>
-      </c>
-      <c r="P14" s="10">
-        <v>233</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="R14" s="10">
-        <v>2</v>
-      </c>
-      <c r="S14" s="11">
-        <v>233</v>
-      </c>
-      <c r="T14" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="U14" s="11">
-        <v>233</v>
-      </c>
-      <c r="V14" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1459,35 +980,15 @@
         <v>8</v>
       </c>
       <c r="H15" s="6">
-        <f>IF(F15&lt;&gt;"",$B15,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I15" s="7">
-        <f>IF(G15&lt;&gt;"",$B15,"")</f>
-        <v>3</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="O15" s="1">
-        <f>SUM(M4:O14)</f>
-        <v>3795</v>
-      </c>
-      <c r="P15" s="6"/>
-      <c r="R15" s="1">
-        <f>SUM(P4:R14)</f>
-        <v>2661</v>
-      </c>
-      <c r="S15" s="6"/>
-      <c r="T15" s="1">
-        <f>SUM(S4:T14)</f>
-        <v>1023</v>
-      </c>
-      <c r="U15" s="6"/>
-      <c r="V15" s="1">
-        <f>SUM(U4:V14)</f>
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1510,11 +1011,11 @@
         <v>8</v>
       </c>
       <c r="H16" s="6">
-        <f>IF(F16&lt;&gt;"",$B16,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I16" s="7">
-        <f>IF(G16&lt;&gt;"",$B16,"")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1539,11 +1040,11 @@
         <v>8</v>
       </c>
       <c r="H17" s="6" t="str">
-        <f>IF(F17&lt;&gt;"",$B17,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I17" s="7">
-        <f>IF(G17&lt;&gt;"",$B17,"")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1570,11 +1071,11 @@
         <v>8</v>
       </c>
       <c r="H18" s="6">
-        <f>IF(F18&lt;&gt;"",$B18,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I18" s="7">
-        <f>IF(G18&lt;&gt;"",$B18,"")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1601,11 +1102,11 @@
         <v>8</v>
       </c>
       <c r="H19" s="6">
-        <f>IF(F19&lt;&gt;"",$B19,"")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I19" s="7">
-        <f>IF(G19&lt;&gt;"",$B19,"")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1630,11 +1131,11 @@
         <v>8</v>
       </c>
       <c r="H20" s="6" t="str">
-        <f>IF(F20&lt;&gt;"",$B20,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I20" s="7">
-        <f>IF(G20&lt;&gt;"",$B20,"")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1661,11 +1162,11 @@
         <v>8</v>
       </c>
       <c r="H21" s="6">
-        <f>IF(F21&lt;&gt;"",$B21,"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I21" s="7">
-        <f>IF(G21&lt;&gt;"",$B21,"")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1692,11 +1193,11 @@
         <v>8</v>
       </c>
       <c r="H22" s="6">
-        <f>IF(F22&lt;&gt;"",$B22,"")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I22" s="7">
-        <f>IF(G22&lt;&gt;"",$B22,"")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1723,17 +1224,17 @@
         <v>8</v>
       </c>
       <c r="H23" s="6">
-        <f>IF(F23&lt;&gt;"",$B23,"")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I23" s="7">
-        <f>IF(G23&lt;&gt;"",$B23,"")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
@@ -1752,17 +1253,17 @@
         <v>8</v>
       </c>
       <c r="H24" s="6" t="str">
-        <f>IF(F24&lt;&gt;"",$B24,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I24" s="7">
-        <f>IF(G24&lt;&gt;"",$B24,"")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -1781,11 +1282,11 @@
         <v>8</v>
       </c>
       <c r="H25" s="6" t="str">
-        <f>IF(F25&lt;&gt;"",$B25,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I25" s="7">
-        <f>IF(G25&lt;&gt;"",$B25,"")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1810,17 +1311,17 @@
         <v>8</v>
       </c>
       <c r="H26" s="6" t="str">
-        <f>IF(F26&lt;&gt;"",$B26,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I26" s="7">
-        <f>IF(G26&lt;&gt;"",$B26,"")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
@@ -1839,11 +1340,11 @@
         <v>8</v>
       </c>
       <c r="H27" s="6" t="str">
-        <f>IF(F27&lt;&gt;"",$B27,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I27" s="7">
-        <f>IF(G27&lt;&gt;"",$B27,"")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1868,63 +1369,58 @@
         <v>8</v>
       </c>
       <c r="H28" s="6" t="str">
-        <f>IF(F28&lt;&gt;"",$B28,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I28" s="7">
-        <f>IF(G28&lt;&gt;"",$B28,"")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="8">
         <v>5</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="10">
-        <v>11</v>
-      </c>
-      <c r="E29" s="10" t="s">
+      <c r="C29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="8">
+        <v>11</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="11" t="str">
-        <f>IF(F29&lt;&gt;"",$B29,"")</f>
+      <c r="F29" s="9"/>
+      <c r="G29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="9" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I29" s="10">
-        <f>IF(G29&lt;&gt;"",$B29,"")</f>
+      <c r="I29" s="8">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="18">
+      <c r="H30" s="10">
         <f>SUM(H4:H29)</f>
         <v>233</v>
       </c>
-      <c r="I30" s="19">
+      <c r="I30" s="11">
         <f>SUM(I4:I29)</f>
         <v>162</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="U2:V2"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:V1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
   </mergeCells>

</xml_diff>